<commit_message>
ran script on new data
</commit_message>
<xml_diff>
--- a/pH_optode/RWS_01_11.xlsx
+++ b/pH_optode/RWS_01_11.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://joinnioz-my.sharepoint.com/personal/louise_delaigue_nioz_nl/Documents/_LAB/RWS/2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="193" documentId="8_{0985D069-2439-40B4-A76B-47398E5EA00A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{40F9646E-EEB7-4F9A-B34B-59B3B8EE11BE}"/>
+  <xr:revisionPtr revIDLastSave="483" documentId="8_{0985D069-2439-40B4-A76B-47398E5EA00A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EDC055FC-B21C-47AC-87B2-74BF14F148EE}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{AFFA04B0-61ED-42A2-921A-E115E7B57E02}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AFFA04B0-61ED-42A2-921A-E115E7B57E02}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="94">
   <si>
     <t>sample</t>
   </si>
@@ -59,15 +59,9 @@
     <t>#</t>
   </si>
   <si>
-    <t>analysis date</t>
-  </si>
-  <si>
     <t>loc</t>
   </si>
   <si>
-    <t>bottled date</t>
-  </si>
-  <si>
     <t>pH_optN</t>
   </si>
   <si>
@@ -192,18 +186,150 @@
   </si>
   <si>
     <t>2020-09-10_172708_CRM2</t>
+  </si>
+  <si>
+    <t>15/09/2020</t>
+  </si>
+  <si>
+    <t>pH_CRM_calc</t>
+  </si>
+  <si>
+    <t>186-0196</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>k1k2_sulpis_borate_uppstrom</t>
+  </si>
+  <si>
+    <t>186-0515</t>
+  </si>
+  <si>
+    <t>2020-09-15_102619_CRM1</t>
+  </si>
+  <si>
+    <t>2020-09-15_104319_WALCRN70_2020005961</t>
+  </si>
+  <si>
+    <t>WALCRN70</t>
+  </si>
+  <si>
+    <t>2020-09-15_110822_NOORDWK70_2020005968</t>
+  </si>
+  <si>
+    <t>2020-09-15_113335_NOORDWK10_2020005966</t>
+  </si>
+  <si>
+    <t>NOORDWK10</t>
+  </si>
+  <si>
+    <t>NOORDWK70</t>
+  </si>
+  <si>
+    <t>2020-09-15_115755_GOERE2_2020005963</t>
+  </si>
+  <si>
+    <t>GOERE2</t>
+  </si>
+  <si>
+    <t>2020-09-15_122345_WALCRN2_2020005959</t>
+  </si>
+  <si>
+    <t>WALCRN2</t>
+  </si>
+  <si>
+    <t>2020-09-15_124748_NOORDWK2_2020005965</t>
+  </si>
+  <si>
+    <t>NOORDWK2</t>
+  </si>
+  <si>
+    <t>2020-09-15_131320_SCHOUWN10_2020005962</t>
+  </si>
+  <si>
+    <t>SCHOUWN10</t>
+  </si>
+  <si>
+    <t>2020-09-15_133821_NOORDWK2_2020004017</t>
+  </si>
+  <si>
+    <t>2020-09-15_140233_WALCRN2_2020004011</t>
+  </si>
+  <si>
+    <t>2020-09-15_142745_NOORDWK70_2020004020</t>
+  </si>
+  <si>
+    <t>2020-09-15_145318_WALCRN70_2020004013</t>
+  </si>
+  <si>
+    <t>2020-09-15_151800_NOORDWK10_2020004018</t>
+  </si>
+  <si>
+    <t>2020-09-15_154239_TERSLG50_2020004022</t>
+  </si>
+  <si>
+    <t>2020-09-15_160630_NOORDWK20_2020004019</t>
+  </si>
+  <si>
+    <t>2020-09-15_163010_TERSLG10_2020004021</t>
+  </si>
+  <si>
+    <t>2020-09-15_165314_CRM2</t>
+  </si>
+  <si>
+    <t>2020-09-16_102128_CRM1</t>
+  </si>
+  <si>
+    <t>16/09/2020</t>
+  </si>
+  <si>
+    <t>186-0809</t>
+  </si>
+  <si>
+    <t>2020-09-16_103737_GOERE6_2020004016</t>
+  </si>
+  <si>
+    <t>2020-09-16_110016_SCHOUWN10_2020004014</t>
+  </si>
+  <si>
+    <t>2020-09-16_112313_WALCRN20_2020004012</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>2020-09-16_121738_GOERE2_2020004015</t>
+  </si>
+  <si>
+    <t>time_to_eq</t>
+  </si>
+  <si>
+    <t>analysis_date</t>
+  </si>
+  <si>
+    <t>bottled_date</t>
+  </si>
+  <si>
+    <t>2020-09-16_125016_NOORDWK20_2020003075</t>
+  </si>
+  <si>
+    <t>2020-09-16_132252_NOORDWK2_2020003073</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yyyy;@"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="0.0000"/>
+    <numFmt numFmtId="168" formatCode="0.000000"/>
+    <numFmt numFmtId="169" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -334,6 +460,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -680,7 +812,7 @@
     <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -729,6 +861,45 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1084,31 +1255,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24354337-39CE-416A-A127-42BEC72437C4}">
-  <dimension ref="A1:P18"/>
+  <dimension ref="A1:R41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L42" sqref="L42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="15.26953125" customWidth="1"/>
-    <col min="3" max="3" width="10.7265625" customWidth="1"/>
+    <col min="3" max="3" width="15.54296875" customWidth="1"/>
+    <col min="4" max="4" width="17.54296875" customWidth="1"/>
     <col min="5" max="5" width="16.7265625" customWidth="1"/>
     <col min="9" max="9" width="10.7265625" style="11"/>
-    <col min="12" max="12" width="10.7265625" style="12"/>
-    <col min="15" max="15" width="19.453125" customWidth="1"/>
+    <col min="10" max="10" width="10.7265625" style="21"/>
+    <col min="12" max="12" width="10.7265625" style="30"/>
+    <col min="14" max="14" width="10.7265625" style="12"/>
+    <col min="17" max="17" width="19.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -1120,42 +1295,48 @@
         <v>2</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="J1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="N1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A2" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A2" s="14" t="s">
-        <v>15</v>
-      </c>
       <c r="B2" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>7</v>
@@ -1170,44 +1351,50 @@
         <v>6</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I2" s="8"/>
-      <c r="J2" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L2" s="13"/>
+      <c r="J2" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>87</v>
+      </c>
       <c r="M2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>17</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="N2" s="13"/>
       <c r="O2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B3" s="16">
         <v>44113</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="13">
-        <v>186</v>
+        <v>18</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>53</v>
       </c>
       <c r="E3" s="10">
         <v>21.1</v>
@@ -1221,27 +1408,33 @@
       <c r="H3" s="12">
         <v>53.029198000000001</v>
       </c>
-      <c r="I3" s="12">
+      <c r="I3" s="20">
         <v>-0.36194900000000002</v>
       </c>
-      <c r="J3" s="7">
+      <c r="J3" s="8">
+        <v>7.9596149896060702</v>
+      </c>
+      <c r="K3" s="7">
         <v>7.96</v>
       </c>
-      <c r="K3" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="L3" s="15"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
+      <c r="L3" s="7">
+        <v>20</v>
+      </c>
+      <c r="M3" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="N3" s="15"/>
       <c r="O3" s="13"/>
       <c r="P3" s="13"/>
-    </row>
-    <row r="4" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="Q3" s="13"/>
+      <c r="R3" s="13"/>
+    </row>
+    <row r="4" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B4" s="9">
         <v>44113</v>
       </c>
-      <c r="C4" s="15" t="s">
-        <v>22</v>
+      <c r="C4" s="25" t="s">
+        <v>20</v>
       </c>
       <c r="D4" s="2">
         <v>2020005969</v>
@@ -1258,23 +1451,29 @@
       <c r="H4" s="11">
         <v>53.029198000000001</v>
       </c>
-      <c r="I4" s="12">
+      <c r="I4" s="20">
         <v>-0.36194900000000002</v>
       </c>
-      <c r="J4" s="13">
+      <c r="J4" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="K4" s="13">
         <v>8.06</v>
       </c>
-      <c r="K4" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="L4" s="15"/>
-    </row>
-    <row r="5" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="L4" s="7">
+        <v>20</v>
+      </c>
+      <c r="M4" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="N4" s="15"/>
+    </row>
+    <row r="5" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B5" s="16">
         <v>44113</v>
       </c>
-      <c r="C5" s="15" t="s">
-        <v>23</v>
+      <c r="C5" s="25" t="s">
+        <v>21</v>
       </c>
       <c r="D5" s="13">
         <v>2020005970</v>
@@ -1291,25 +1490,31 @@
       <c r="H5" s="12">
         <v>53.029198000000001</v>
       </c>
-      <c r="I5" s="12">
+      <c r="I5" s="20">
         <v>-0.36194900000000002</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="K5" s="2">
         <v>8.0500000000000007</v>
       </c>
-      <c r="K5" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="L5" s="15"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
-    </row>
-    <row r="6" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="L5" s="7">
+        <v>20</v>
+      </c>
+      <c r="M5" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="N5" s="15"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="12"/>
+    </row>
+    <row r="6" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B6" s="16">
         <v>44113</v>
       </c>
-      <c r="C6" s="15" t="s">
-        <v>27</v>
+      <c r="C6" s="25" t="s">
+        <v>25</v>
       </c>
       <c r="D6" s="13">
         <v>2020005971</v>
@@ -1326,23 +1531,29 @@
       <c r="H6" s="12">
         <v>53.029198000000001</v>
       </c>
-      <c r="I6" s="12">
+      <c r="I6" s="20">
         <v>-0.36194900000000002</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="K6" s="2">
         <v>8.0299999999999994</v>
       </c>
-      <c r="K6" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="L6" s="15"/>
-    </row>
-    <row r="7" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="L6" s="7">
+        <v>20</v>
+      </c>
+      <c r="M6" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="N6" s="15"/>
+    </row>
+    <row r="7" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B7" s="16">
         <v>44113</v>
       </c>
-      <c r="C7" s="15" t="s">
-        <v>28</v>
+      <c r="C7" s="25" t="s">
+        <v>26</v>
       </c>
       <c r="D7" s="13">
         <v>2020005972</v>
@@ -1359,25 +1570,31 @@
       <c r="H7" s="12">
         <v>53.029198000000001</v>
       </c>
-      <c r="I7" s="12">
+      <c r="I7" s="20">
         <v>-0.36194900000000002</v>
       </c>
-      <c r="J7" s="2">
+      <c r="J7" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="K7" s="2">
         <v>7.98</v>
       </c>
-      <c r="K7" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
+      <c r="L7" s="7">
+        <v>20</v>
+      </c>
+      <c r="M7" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="N7" s="12"/>
-    </row>
-    <row r="8" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="O7" s="12"/>
+      <c r="P7" s="12"/>
+    </row>
+    <row r="8" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B8" s="16">
         <v>44113</v>
       </c>
-      <c r="C8" s="15" t="s">
-        <v>30</v>
+      <c r="C8" s="25" t="s">
+        <v>28</v>
       </c>
       <c r="D8" s="13">
         <v>2020005983</v>
@@ -1394,23 +1611,29 @@
       <c r="H8" s="12">
         <v>53.029198000000001</v>
       </c>
-      <c r="I8" s="12">
+      <c r="I8" s="20">
         <v>-0.36194900000000002</v>
       </c>
-      <c r="J8" s="2">
+      <c r="J8" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="K8" s="2">
         <v>7.95</v>
       </c>
-      <c r="K8" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="L8" s="15"/>
-    </row>
-    <row r="9" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="L8" s="7">
+        <v>20</v>
+      </c>
+      <c r="M8" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="N8" s="15"/>
+    </row>
+    <row r="9" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B9" s="16">
         <v>44113</v>
       </c>
-      <c r="C9" s="15" t="s">
-        <v>30</v>
+      <c r="C9" s="25" t="s">
+        <v>28</v>
       </c>
       <c r="D9" s="13">
         <v>2020005973</v>
@@ -1427,23 +1650,29 @@
       <c r="H9" s="12">
         <v>53.029198000000001</v>
       </c>
-      <c r="I9" s="12">
+      <c r="I9" s="20">
         <v>-0.36194900000000002</v>
       </c>
-      <c r="J9" s="2">
+      <c r="J9" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="K9" s="2">
         <v>7.95</v>
       </c>
-      <c r="K9" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="L9" s="15"/>
-    </row>
-    <row r="10" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="L9" s="7">
+        <v>20</v>
+      </c>
+      <c r="M9" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="N9" s="15"/>
+    </row>
+    <row r="10" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B10" s="16">
         <v>44113</v>
       </c>
-      <c r="C10" s="15" t="s">
-        <v>33</v>
+      <c r="C10" s="25" t="s">
+        <v>31</v>
       </c>
       <c r="D10" s="13">
         <v>2020005976</v>
@@ -1460,23 +1689,29 @@
       <c r="H10" s="12">
         <v>53.029198000000001</v>
       </c>
-      <c r="I10" s="12">
+      <c r="I10" s="20">
         <v>-0.36194900000000002</v>
       </c>
-      <c r="J10" s="2">
+      <c r="J10" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="K10" s="2">
         <v>8.0500000000000007</v>
       </c>
-      <c r="K10" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="L10" s="15"/>
-    </row>
-    <row r="11" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="L10" s="7">
+        <v>20</v>
+      </c>
+      <c r="M10" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="N10" s="15"/>
+    </row>
+    <row r="11" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B11" s="16">
         <v>44113</v>
       </c>
-      <c r="C11" s="15" t="s">
-        <v>30</v>
+      <c r="C11" s="25" t="s">
+        <v>28</v>
       </c>
       <c r="D11" s="13">
         <v>2020005984</v>
@@ -1493,23 +1728,29 @@
       <c r="H11" s="12">
         <v>53.029198000000001</v>
       </c>
-      <c r="I11" s="12">
+      <c r="I11" s="20">
         <v>-0.36194900000000002</v>
       </c>
-      <c r="J11" s="2">
+      <c r="J11" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="K11" s="2">
         <v>7.87</v>
       </c>
-      <c r="K11" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="L11" s="15"/>
-    </row>
-    <row r="12" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="L11" s="7">
+        <v>20</v>
+      </c>
+      <c r="M11" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="N11" s="15"/>
+    </row>
+    <row r="12" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B12" s="16">
         <v>44113</v>
       </c>
-      <c r="C12" s="15" t="s">
-        <v>40</v>
+      <c r="C12" s="25" t="s">
+        <v>38</v>
       </c>
       <c r="D12" s="13">
         <v>2020005974</v>
@@ -1526,23 +1767,29 @@
       <c r="H12" s="12">
         <v>53.029198000000001</v>
       </c>
-      <c r="I12" s="12">
+      <c r="I12" s="20">
         <v>-0.36194900000000002</v>
       </c>
-      <c r="J12" s="2">
+      <c r="J12" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="K12" s="31">
         <v>7.92</v>
       </c>
-      <c r="K12" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="L12" s="15"/>
-    </row>
-    <row r="13" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="L12" s="7">
+        <v>20</v>
+      </c>
+      <c r="M12" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="N12" s="15"/>
+    </row>
+    <row r="13" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B13" s="16">
         <v>44113</v>
       </c>
-      <c r="C13" s="15" t="s">
-        <v>42</v>
+      <c r="C13" s="25" t="s">
+        <v>40</v>
       </c>
       <c r="D13" s="13">
         <v>2020005975</v>
@@ -1559,28 +1806,34 @@
       <c r="H13" s="12">
         <v>53.029198000000001</v>
       </c>
-      <c r="I13" s="12">
+      <c r="I13" s="20">
         <v>-0.36194900000000002</v>
       </c>
-      <c r="J13" s="2">
+      <c r="J13" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="K13" s="31">
         <v>8.0500000000000007</v>
       </c>
-      <c r="K13" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="L13" s="17"/>
-      <c r="M13" s="12"/>
-      <c r="N13" s="12"/>
+      <c r="L13" s="7">
+        <v>20</v>
+      </c>
+      <c r="M13" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="N13" s="17"/>
       <c r="O13" s="12"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P13" s="12"/>
+      <c r="Q13" s="12"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B14" s="16">
         <v>44113</v>
       </c>
-      <c r="C14" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14" s="13">
+      <c r="C14" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="25">
         <v>2020005964</v>
       </c>
       <c r="E14" s="10">
@@ -1595,25 +1848,31 @@
       <c r="H14" s="12">
         <v>53.029198000000001</v>
       </c>
-      <c r="I14" s="12">
+      <c r="I14" s="20">
         <v>-0.36194900000000002</v>
       </c>
-      <c r="J14" s="13">
+      <c r="J14" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="K14" s="31">
         <v>8.07</v>
       </c>
-      <c r="K14" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="L14" s="15"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="L14" s="7">
+        <v>20</v>
+      </c>
+      <c r="M14" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="N14" s="15"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B15" s="16">
         <v>44113</v>
       </c>
-      <c r="C15" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="D15" s="13">
+      <c r="C15" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="25">
         <v>2020005967</v>
       </c>
       <c r="E15" s="10">
@@ -1628,25 +1887,31 @@
       <c r="H15" s="12">
         <v>53.029198000000001</v>
       </c>
-      <c r="I15" s="12">
+      <c r="I15" s="20">
         <v>-0.36194900000000002</v>
       </c>
-      <c r="J15" s="13">
+      <c r="J15" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="K15" s="13">
         <v>8.1300000000000008</v>
       </c>
-      <c r="K15" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="L15" s="15"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="L15" s="7">
+        <v>20</v>
+      </c>
+      <c r="M15" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="N15" s="15"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B16" s="16">
         <v>44113</v>
       </c>
-      <c r="C16" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="D16" s="13">
+      <c r="C16" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="25">
         <v>2020005960</v>
       </c>
       <c r="E16" s="10">
@@ -1661,28 +1926,37 @@
       <c r="H16" s="12">
         <v>53.029198000000001</v>
       </c>
-      <c r="I16" s="12">
+      <c r="I16" s="20">
         <v>-0.36194900000000002</v>
       </c>
-      <c r="J16" s="13">
+      <c r="J16" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="K16" s="31">
         <v>7.83</v>
       </c>
-      <c r="K16" s="15" t="s">
+      <c r="L16" s="7">
+        <v>20</v>
+      </c>
+      <c r="M16" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="N16" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="L16" s="15" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A17" s="25" t="s">
+        <v>23</v>
+      </c>
       <c r="B17" s="16">
         <v>44113</v>
       </c>
-      <c r="C17" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="13">
-        <v>186</v>
+      <c r="C17" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="25" t="s">
+        <v>53</v>
       </c>
       <c r="E17" s="10">
         <v>21.1</v>
@@ -1696,22 +1970,949 @@
       <c r="H17" s="12">
         <v>53.029198000000001</v>
       </c>
-      <c r="I17" s="12">
+      <c r="I17" s="20">
         <v>-0.36194900000000002</v>
       </c>
-      <c r="J17" s="13">
+      <c r="J17" s="8">
+        <v>7.9596149896060702</v>
+      </c>
+      <c r="K17" s="31">
         <v>7.86</v>
       </c>
-      <c r="K17" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="L17" s="15"/>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="K18" s="15"/>
-      <c r="L18" s="15"/>
+      <c r="L17" s="7">
+        <v>20</v>
+      </c>
+      <c r="M17" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="N17" s="15"/>
+    </row>
+    <row r="18" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="E18" s="10">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="F18" s="10">
+        <v>20</v>
+      </c>
+      <c r="G18" s="24">
+        <v>24.265301000000001</v>
+      </c>
+      <c r="H18" s="24">
+        <v>53.051501999999999</v>
+      </c>
+      <c r="I18" s="20">
+        <v>-0.36425000000000002</v>
+      </c>
+      <c r="J18" s="8">
+        <v>7.9596149896060702</v>
+      </c>
+      <c r="K18" s="31">
+        <v>7.96</v>
+      </c>
+      <c r="L18" s="7">
+        <v>20</v>
+      </c>
+      <c r="M18" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="N18" s="15"/>
+    </row>
+    <row r="19" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" s="25">
+        <v>2020005961</v>
+      </c>
+      <c r="E19" s="10">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="F19" s="10">
+        <v>20</v>
+      </c>
+      <c r="G19" s="24">
+        <v>24.265301000000001</v>
+      </c>
+      <c r="H19" s="24">
+        <v>53.051501999999999</v>
+      </c>
+      <c r="I19" s="20">
+        <v>-0.36425000000000002</v>
+      </c>
+      <c r="J19" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="K19" s="31">
+        <v>8.0500000000000007</v>
+      </c>
+      <c r="L19" s="7">
+        <v>20</v>
+      </c>
+      <c r="M19" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="N19" s="15"/>
+    </row>
+    <row r="20" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="D20" s="25">
+        <v>2020005968</v>
+      </c>
+      <c r="E20" s="10">
+        <v>21.3</v>
+      </c>
+      <c r="F20" s="10">
+        <v>20</v>
+      </c>
+      <c r="G20" s="24">
+        <v>24.265301000000001</v>
+      </c>
+      <c r="H20" s="24">
+        <v>53.051501999999999</v>
+      </c>
+      <c r="I20" s="20">
+        <v>-0.36425000000000002</v>
+      </c>
+      <c r="J20" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="K20" s="31">
+        <v>8.01</v>
+      </c>
+      <c r="L20" s="7">
+        <v>20</v>
+      </c>
+      <c r="M20" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="N20" s="15"/>
+    </row>
+    <row r="21" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="D21" s="25">
+        <v>2020005966</v>
+      </c>
+      <c r="E21" s="10">
+        <v>20.5</v>
+      </c>
+      <c r="F21" s="10">
+        <v>20</v>
+      </c>
+      <c r="G21" s="24">
+        <v>24.265301000000001</v>
+      </c>
+      <c r="H21" s="24">
+        <v>53.051501999999999</v>
+      </c>
+      <c r="I21" s="20">
+        <v>-0.36425000000000002</v>
+      </c>
+      <c r="J21" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="K21" s="31">
+        <v>8.11</v>
+      </c>
+      <c r="L21" s="7">
+        <v>20</v>
+      </c>
+      <c r="M21" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="N21" s="15"/>
+    </row>
+    <row r="22" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" s="25">
+        <v>2020005963</v>
+      </c>
+      <c r="E22" s="10">
+        <v>20.7</v>
+      </c>
+      <c r="F22" s="10">
+        <v>20</v>
+      </c>
+      <c r="G22" s="24">
+        <v>24.265301000000001</v>
+      </c>
+      <c r="H22" s="24">
+        <v>53.051501999999999</v>
+      </c>
+      <c r="I22" s="20">
+        <v>-0.36425000000000002</v>
+      </c>
+      <c r="J22" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="K22" s="31">
+        <v>8.06</v>
+      </c>
+      <c r="L22" s="7">
+        <v>20</v>
+      </c>
+      <c r="M22" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="N22" s="15"/>
+    </row>
+    <row r="23" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="D23" s="25">
+        <v>2020005959</v>
+      </c>
+      <c r="E23" s="10">
+        <v>20.7</v>
+      </c>
+      <c r="F23" s="10">
+        <v>20</v>
+      </c>
+      <c r="G23" s="24">
+        <v>24.265301000000001</v>
+      </c>
+      <c r="H23" s="24">
+        <v>53.051501999999999</v>
+      </c>
+      <c r="I23" s="20">
+        <v>-0.36425000000000002</v>
+      </c>
+      <c r="J23" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="K23" s="31">
+        <v>8.0500000000000007</v>
+      </c>
+      <c r="L23" s="7">
+        <v>20</v>
+      </c>
+      <c r="M23" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="N23" s="15"/>
+    </row>
+    <row r="24" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="D24" s="25">
+        <v>2020005965</v>
+      </c>
+      <c r="E24" s="10">
+        <v>20.6</v>
+      </c>
+      <c r="F24" s="10">
+        <v>20</v>
+      </c>
+      <c r="G24" s="24">
+        <v>24.265301000000001</v>
+      </c>
+      <c r="H24" s="24">
+        <v>53.051501999999999</v>
+      </c>
+      <c r="I24" s="20">
+        <v>-0.36425000000000002</v>
+      </c>
+      <c r="J24" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="K24" s="31">
+        <v>8.02</v>
+      </c>
+      <c r="L24" s="7">
+        <v>20</v>
+      </c>
+      <c r="M24" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="N24" s="15"/>
+    </row>
+    <row r="25" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="D25" s="25">
+        <v>2020005962</v>
+      </c>
+      <c r="E25" s="10">
+        <v>20.7</v>
+      </c>
+      <c r="F25" s="10">
+        <v>20</v>
+      </c>
+      <c r="G25" s="24">
+        <v>24.265301000000001</v>
+      </c>
+      <c r="H25" s="24">
+        <v>53.051501999999999</v>
+      </c>
+      <c r="I25" s="20">
+        <v>-0.36425000000000002</v>
+      </c>
+      <c r="J25" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="K25" s="31">
+        <v>8.0399999999999991</v>
+      </c>
+      <c r="L25" s="7">
+        <v>20</v>
+      </c>
+      <c r="M25" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="N25" s="15"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B26" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="D26" s="25">
+        <v>2020004017</v>
+      </c>
+      <c r="E26" s="10">
+        <v>19.8</v>
+      </c>
+      <c r="F26" s="10">
+        <v>20</v>
+      </c>
+      <c r="G26" s="24">
+        <v>24.265301000000001</v>
+      </c>
+      <c r="H26" s="24">
+        <v>53.051501999999999</v>
+      </c>
+      <c r="I26" s="20">
+        <v>-0.36425000000000002</v>
+      </c>
+      <c r="J26" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="K26" s="31">
+        <v>7.79</v>
+      </c>
+      <c r="L26" s="7">
+        <v>20</v>
+      </c>
+      <c r="M26" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B27" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="D27" s="25">
+        <v>2020004011</v>
+      </c>
+      <c r="E27" s="10">
+        <v>20.3</v>
+      </c>
+      <c r="F27" s="10">
+        <v>20</v>
+      </c>
+      <c r="G27" s="24">
+        <v>24.265301000000001</v>
+      </c>
+      <c r="H27" s="24">
+        <v>53.051501999999999</v>
+      </c>
+      <c r="I27" s="20">
+        <v>-0.36425000000000002</v>
+      </c>
+      <c r="J27" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="K27" s="7">
+        <v>7.8</v>
+      </c>
+      <c r="L27" s="7">
+        <v>20</v>
+      </c>
+      <c r="M27" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B28" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="D28" s="25">
+        <v>2020004020</v>
+      </c>
+      <c r="E28" s="10">
+        <v>20.6</v>
+      </c>
+      <c r="F28" s="10">
+        <v>20</v>
+      </c>
+      <c r="G28" s="24">
+        <v>24.265301000000001</v>
+      </c>
+      <c r="H28" s="24">
+        <v>53.051501999999999</v>
+      </c>
+      <c r="I28" s="20">
+        <v>-0.36425000000000002</v>
+      </c>
+      <c r="J28" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="K28" s="31">
+        <v>7.9</v>
+      </c>
+      <c r="L28" s="7">
+        <v>20</v>
+      </c>
+      <c r="M28" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B29" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C29" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="D29" s="25">
+        <v>2020004013</v>
+      </c>
+      <c r="E29" s="10">
+        <v>20</v>
+      </c>
+      <c r="F29" s="10">
+        <v>20</v>
+      </c>
+      <c r="G29" s="24">
+        <v>24.265301000000001</v>
+      </c>
+      <c r="H29" s="24">
+        <v>53.051501999999999</v>
+      </c>
+      <c r="I29" s="20">
+        <v>-0.36425000000000002</v>
+      </c>
+      <c r="J29" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="K29" s="31">
+        <v>7.91</v>
+      </c>
+      <c r="L29" s="7">
+        <v>20</v>
+      </c>
+      <c r="M29" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B30" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="D30" s="25">
+        <v>2020004018</v>
+      </c>
+      <c r="E30" s="10">
+        <v>21.3</v>
+      </c>
+      <c r="F30" s="10">
+        <v>20</v>
+      </c>
+      <c r="G30" s="24">
+        <v>24.265301000000001</v>
+      </c>
+      <c r="H30" s="24">
+        <v>53.051501999999999</v>
+      </c>
+      <c r="I30" s="20">
+        <v>-0.36425000000000002</v>
+      </c>
+      <c r="J30" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="K30" s="31">
+        <v>7.81</v>
+      </c>
+      <c r="L30" s="7">
+        <v>20</v>
+      </c>
+      <c r="M30" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B31" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C31" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31" s="25">
+        <v>2020004022</v>
+      </c>
+      <c r="E31" s="10">
+        <v>20.6</v>
+      </c>
+      <c r="F31" s="10">
+        <v>20</v>
+      </c>
+      <c r="G31" s="24">
+        <v>24.265301000000001</v>
+      </c>
+      <c r="H31" s="24">
+        <v>53.051501999999999</v>
+      </c>
+      <c r="I31" s="20">
+        <v>-0.36425000000000002</v>
+      </c>
+      <c r="J31" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="K31" s="31">
+        <v>7.85</v>
+      </c>
+      <c r="L31" s="7">
+        <v>20</v>
+      </c>
+      <c r="M31" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B32" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C32" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="D32" s="25">
+        <v>2020004019</v>
+      </c>
+      <c r="E32" s="10">
+        <v>20.3</v>
+      </c>
+      <c r="F32" s="10">
+        <v>20</v>
+      </c>
+      <c r="G32" s="24">
+        <v>24.265301000000001</v>
+      </c>
+      <c r="H32" s="24">
+        <v>53.051501999999999</v>
+      </c>
+      <c r="I32" s="20">
+        <v>-0.36425000000000002</v>
+      </c>
+      <c r="J32" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="K32" s="31">
+        <v>7.87</v>
+      </c>
+      <c r="L32" s="7">
+        <v>20</v>
+      </c>
+      <c r="M32" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B33" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C33" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="D33" s="25">
+        <v>2020004021</v>
+      </c>
+      <c r="E33" s="10">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="F33" s="10">
+        <v>20</v>
+      </c>
+      <c r="G33" s="24">
+        <v>24.265301000000001</v>
+      </c>
+      <c r="H33" s="24">
+        <v>53.051501999999999</v>
+      </c>
+      <c r="I33" s="20">
+        <v>-0.36425000000000002</v>
+      </c>
+      <c r="J33" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="K33" s="31">
+        <v>7.88</v>
+      </c>
+      <c r="L33" s="7">
+        <v>20</v>
+      </c>
+      <c r="M33" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A34" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="B34" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C34" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="D34" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="E34" s="10">
+        <v>20</v>
+      </c>
+      <c r="F34" s="10">
+        <v>20</v>
+      </c>
+      <c r="G34" s="24">
+        <v>24.265301000000001</v>
+      </c>
+      <c r="H34" s="24">
+        <v>53.051501999999999</v>
+      </c>
+      <c r="I34" s="20">
+        <v>-0.36425000000000002</v>
+      </c>
+      <c r="J34" s="8">
+        <v>7.9596149896060702</v>
+      </c>
+      <c r="K34" s="31">
+        <v>7.95</v>
+      </c>
+      <c r="L34" s="7">
+        <v>20</v>
+      </c>
+      <c r="M34" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A35" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="C35" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="D35" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="E35" s="10">
+        <v>19.8</v>
+      </c>
+      <c r="F35" s="10">
+        <v>20</v>
+      </c>
+      <c r="G35" s="29">
+        <v>24.353750000000002</v>
+      </c>
+      <c r="H35" s="29">
+        <v>53.057445999999999</v>
+      </c>
+      <c r="I35" s="34">
+        <v>-0.3548</v>
+      </c>
+      <c r="J35" s="8">
+        <v>7.9596149896060702</v>
+      </c>
+      <c r="K35" s="31">
+        <v>7.96</v>
+      </c>
+      <c r="L35" s="7">
+        <v>20</v>
+      </c>
+      <c r="M35" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B36" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="C36" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="D36" s="25">
+        <v>2020004016</v>
+      </c>
+      <c r="E36" s="10">
+        <v>20.5</v>
+      </c>
+      <c r="F36" s="10">
+        <v>20</v>
+      </c>
+      <c r="G36" s="30">
+        <v>24.353750000000002</v>
+      </c>
+      <c r="H36" s="30">
+        <v>53.057445999999999</v>
+      </c>
+      <c r="I36" s="34">
+        <v>-0.3548</v>
+      </c>
+      <c r="J36" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="K36" s="31">
+        <v>7.8</v>
+      </c>
+      <c r="L36" s="7">
+        <v>20</v>
+      </c>
+      <c r="M36" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B37" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="C37" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="D37" s="31">
+        <v>2020004014</v>
+      </c>
+      <c r="E37" s="10">
+        <v>20</v>
+      </c>
+      <c r="F37" s="10">
+        <v>20</v>
+      </c>
+      <c r="G37" s="30">
+        <v>24.353750000000002</v>
+      </c>
+      <c r="H37" s="30">
+        <v>53.057445999999999</v>
+      </c>
+      <c r="I37" s="34">
+        <v>-0.3548</v>
+      </c>
+      <c r="J37" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="K37" s="31">
+        <v>7.83</v>
+      </c>
+      <c r="L37" s="7">
+        <v>20</v>
+      </c>
+      <c r="M37" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B38" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="C38" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="D38" s="31">
+        <v>2020004012</v>
+      </c>
+      <c r="E38" s="10">
+        <v>20</v>
+      </c>
+      <c r="F38" s="10">
+        <v>20</v>
+      </c>
+      <c r="G38" s="30">
+        <v>24.353750000000002</v>
+      </c>
+      <c r="H38" s="30">
+        <v>53.057445999999999</v>
+      </c>
+      <c r="I38" s="34">
+        <v>-0.3548</v>
+      </c>
+      <c r="J38" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="K38" s="31">
+        <v>7.94</v>
+      </c>
+      <c r="L38" s="7">
+        <v>30</v>
+      </c>
+      <c r="M38" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B39" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="C39" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="D39" s="31">
+        <v>2020004015</v>
+      </c>
+      <c r="E39" s="10">
+        <v>21.3</v>
+      </c>
+      <c r="F39" s="10">
+        <v>20</v>
+      </c>
+      <c r="G39" s="30">
+        <v>24.353750000000002</v>
+      </c>
+      <c r="H39" s="30">
+        <v>53.057445999999999</v>
+      </c>
+      <c r="I39" s="34">
+        <v>-0.3548</v>
+      </c>
+      <c r="J39" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="K39" s="7">
+        <v>7.8</v>
+      </c>
+      <c r="L39" s="7">
+        <v>30</v>
+      </c>
+      <c r="M39" s="28" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B40" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="C40" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="D40" s="31">
+        <v>2020003075</v>
+      </c>
+      <c r="E40" s="10">
+        <v>21</v>
+      </c>
+      <c r="F40" s="10">
+        <v>20</v>
+      </c>
+      <c r="G40" s="30">
+        <v>24.353750000000002</v>
+      </c>
+      <c r="H40" s="30">
+        <v>53.057445999999999</v>
+      </c>
+      <c r="I40" s="34">
+        <v>-0.3548</v>
+      </c>
+      <c r="J40" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="K40" s="7">
+        <v>7.8</v>
+      </c>
+      <c r="L40" s="7">
+        <v>30</v>
+      </c>
+      <c r="M40" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B41" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="C41" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="D41" s="31">
+        <v>2020003073</v>
+      </c>
+      <c r="F41" s="10">
+        <v>20</v>
+      </c>
+      <c r="G41" s="30">
+        <v>24.353750000000002</v>
+      </c>
+      <c r="H41" s="30">
+        <v>53.057445999999999</v>
+      </c>
+      <c r="I41" s="34">
+        <v>-0.3548</v>
+      </c>
+      <c r="J41" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="K41" s="31"/>
+      <c r="L41" s="7">
+        <v>30</v>
+      </c>
+      <c r="M41" t="s">
+        <v>93</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>